<commit_message>
j'en suis au download repport
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uipath-my.sharepoint.com/personal/alexandra_veizu_uipath_com/Documents/Documents/Projects/FrameworkTemplates/REFramework/VB/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://positivethinkingcompany-my.sharepoint.com/personal/qcacciatore_positivethinking_tech/Documents/Documents/UiPath/GenerateYearlyReport_Performer/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{00D541BD-CB78-4D75-8532-9AD73E8C785E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{F8C54E24-BA5C-4BF9-8DAB-2778512EC11B}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{00D541BD-CB78-4D75-8532-9AD73E8C785E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6E8DFD2F-FD56-4140-B6C5-BDFB29246EB8}"/>
   <bookViews>
-    <workbookView xWindow="-10248" yWindow="17508" windowWidth="21252" windowHeight="9444" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="48">
   <si>
     <t>Name</t>
   </si>
@@ -159,14 +159,23 @@
     <t xml:space="preserve">The maximum number of consecutive system exceptions was reached. </t>
   </si>
   <si>
-    <t>ProcessABCQueue</t>
+    <t>YearlyReport</t>
+  </si>
+  <si>
+    <t>System1_URL</t>
+  </si>
+  <si>
+    <t>System1_Credential</t>
+  </si>
+  <si>
+    <t>https://acme-test.uipath.com/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -190,6 +199,12 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -208,10 +223,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -221,8 +237,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -239,7 +257,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -538,10 +556,10 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="43.5546875" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
@@ -616,8 +634,22 @@
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="7" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" t="s">
+        <v>46</v>
+      </c>
+    </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1610,8 +1642,11 @@
     <row r="998" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
+  <hyperlinks>
+    <hyperlink ref="B7" r:id="rId1" xr:uid="{EDD5ECEE-A111-4A4C-BBE7-BCF4073E03D9}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1623,7 +1658,7 @@
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
@@ -2786,7 +2821,7 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="31.88671875" customWidth="1"/>
     <col min="2" max="2" width="30.109375" customWidth="1"/>

</xml_diff>